<commit_message>
changed uncertainty of square periods
</commit_message>
<xml_diff>
--- a/graphs/sonar_non-pretensionata_dinamico.xlsx
+++ b/graphs/sonar_non-pretensionata_dinamico.xlsx
@@ -458,10 +458,10 @@
         <v>1.721653791726028</v>
       </c>
       <c r="D2" t="n">
-        <v>0.0003668478529267382</v>
+        <v>0.005</v>
       </c>
       <c r="E2" t="n">
-        <v>0.001159606824447104</v>
+        <v>0.01580442584641887</v>
       </c>
     </row>
     <row r="3">
@@ -475,10 +475,10 @@
         <v>2.493062071715172</v>
       </c>
       <c r="D3" t="n">
-        <v>0.0006571974450906863</v>
+        <v>0.005</v>
       </c>
       <c r="E3" t="n">
-        <v>0.002077349310920983</v>
+        <v>0.01580442584641887</v>
       </c>
     </row>
     <row r="4">
@@ -492,10 +492,10 @@
         <v>3.268023409288708</v>
       </c>
       <c r="D4" t="n">
-        <v>0.0009549276024599289</v>
+        <v>0.005</v>
       </c>
       <c r="E4" t="n">
-        <v>0.003018432457074848</v>
+        <v>0.01580442584641887</v>
       </c>
     </row>
     <row r="5">
@@ -509,10 +509,10 @@
         <v>4.052064782911247</v>
       </c>
       <c r="D5" t="n">
-        <v>0.001299146985731943</v>
+        <v>0.005</v>
       </c>
       <c r="E5" t="n">
-        <v>0.004106465793843366</v>
+        <v>0.01580442584641887</v>
       </c>
     </row>
     <row r="6">
@@ -526,10 +526,10 @@
         <v>4.846765329286962</v>
       </c>
       <c r="D6" t="n">
-        <v>0.001638351812457543</v>
+        <v>0.005</v>
       </c>
       <c r="E6" t="n">
-        <v>0.005178650564458862</v>
+        <v>0.01580442584641887</v>
       </c>
     </row>
   </sheetData>

</xml_diff>